<commit_message>
Vy Nguyen Project Manager role update
</commit_message>
<xml_diff>
--- a/src/test/resources/data/TestData.xlsx
+++ b/src/test/resources/data/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IResource\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168A28E8-2473-48A1-A48B-C4ECF2F47BD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2C102E5-D745-4C22-8245-EFA435B40A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="2" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="118">
   <si>
     <t>Email</t>
   </si>
@@ -373,6 +373,9 @@
   </si>
   <si>
     <t>lily.pham17@mailsac.com</t>
+  </si>
+  <si>
+    <t>vy.nguyen.1@yopmail.com</t>
   </si>
 </sst>
 </file>
@@ -976,6 +979,7 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="8" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -994,7 +998,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1353,8 +1356,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE7C717B-F1EB-455D-B109-71C9942E3E0E}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1395,7 @@
       <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="D2" s="18" t="s">
         <v>54</v>
       </c>
     </row>
@@ -1406,7 +1409,7 @@
       <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -1418,7 +1421,7 @@
       <c r="C4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="17"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1426,7 +1429,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="17"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
@@ -1438,7 +1441,7 @@
       <c r="C6" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D6" s="17"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1450,7 +1453,7 @@
       <c r="C7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="D7" s="19" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1464,7 +1467,7 @@
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="18"/>
+      <c r="D8" s="19"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1476,7 +1479,7 @@
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="18"/>
+      <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
@@ -1486,7 +1489,7 @@
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="18"/>
+      <c r="D10" s="19"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
@@ -1496,7 +1499,7 @@
         <v>26</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="18"/>
+      <c r="D11" s="19"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1508,7 +1511,7 @@
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="18"/>
+      <c r="D12" s="19"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
@@ -1520,7 +1523,7 @@
       <c r="C13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="20" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1534,7 +1537,7 @@
       <c r="C14" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="19"/>
+      <c r="D14" s="20"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1544,7 +1547,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="19"/>
+      <c r="D15" s="20"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -1554,7 +1557,7 @@
       <c r="C16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="19"/>
+      <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
@@ -1564,7 +1567,7 @@
       <c r="C17" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D17" s="19"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -1609,10 +1612,18 @@
       <c r="A21" t="s">
         <v>45</v>
       </c>
-      <c r="B21" t="s">
-        <v>32</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="B21" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1632,11 +1643,12 @@
     <hyperlink ref="C9" r:id="rId3" xr:uid="{F4C221DA-E540-4F9C-8086-44931846D68C}"/>
     <hyperlink ref="B20" r:id="rId4" xr:uid="{467D1F2F-3AC1-4DB0-81F7-1E7569791FD2}"/>
     <hyperlink ref="C20" r:id="rId5" xr:uid="{22A27956-90B3-41B9-80EB-13613490FEE6}"/>
-    <hyperlink ref="C21" r:id="rId6" xr:uid="{13DA61B5-E342-4D7C-BBB8-5F8A9AC69776}"/>
-    <hyperlink ref="B21" r:id="rId7" xr:uid="{0BE843A8-22DE-4EEF-8C69-E9C370661F31}"/>
+    <hyperlink ref="C21" r:id="rId6" display="mailto:Tuongvy@10" xr:uid="{67811377-A93B-414A-B328-272E65B7817B}"/>
+    <hyperlink ref="B22" r:id="rId7" xr:uid="{BE93581C-516C-41D6-A5E4-D4EB4E017AF1}"/>
+    <hyperlink ref="C22" r:id="rId8" display="mailto:Tuongvy@10" xr:uid="{16B02F66-52EC-4FB6-B958-ABBBA3410ABF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -1644,7 +1656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G129"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
@@ -1693,7 +1705,7 @@
       <c r="C2" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="17" t="s">
         <v>116</v>
       </c>
       <c r="E2" s="14" t="s">
@@ -1702,7 +1714,7 @@
       <c r="F2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="21" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1725,7 +1737,7 @@
       <c r="F3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="21"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
@@ -1740,7 +1752,7 @@
       <c r="D4" s="14"/>
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
-      <c r="G4" s="21"/>
+      <c r="G4" s="22"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
@@ -1755,7 +1767,7 @@
       <c r="D5" s="14"/>
       <c r="E5" s="14"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="21"/>
+      <c r="G5" s="22"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
@@ -1770,7 +1782,7 @@
       <c r="D6" s="14"/>
       <c r="E6" s="14"/>
       <c r="F6" s="14"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
@@ -1785,7 +1797,7 @@
       <c r="D7" s="16"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
-      <c r="G7" s="22"/>
+      <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
@@ -1798,7 +1810,7 @@
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="21" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1821,7 +1833,7 @@
       <c r="F9" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G9" s="21"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
@@ -1834,7 +1846,7 @@
       </c>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -1855,7 +1867,7 @@
       <c r="F11" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="G11" s="21"/>
+      <c r="G11" s="22"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
@@ -1868,7 +1880,7 @@
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
-      <c r="G12" s="21"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
@@ -1887,7 +1899,7 @@
       <c r="F13" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="22"/>
+      <c r="G13" s="23"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
@@ -1900,7 +1912,7 @@
         <v>10</v>
       </c>
       <c r="F14" s="12"/>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1915,7 +1927,7 @@
         <v>98</v>
       </c>
       <c r="F15" s="14"/>
-      <c r="G15" s="21"/>
+      <c r="G15" s="22"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
@@ -1936,7 +1948,7 @@
       <c r="F16" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="G16" s="21"/>
+      <c r="G16" s="22"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
@@ -1955,7 +1967,7 @@
       <c r="F17" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="21"/>
+      <c r="G17" s="22"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="13" t="s">
@@ -1976,7 +1988,7 @@
       <c r="F18" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="21"/>
+      <c r="G18" s="22"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
@@ -1995,7 +2007,7 @@
       <c r="F19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="22"/>
+      <c r="G19" s="23"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
@@ -2010,7 +2022,7 @@
       <c r="F20" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="21" t="s">
         <v>115</v>
       </c>
     </row>
@@ -2027,7 +2039,7 @@
       <c r="F21" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="G21" s="21"/>
+      <c r="G21" s="22"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
@@ -2040,7 +2052,7 @@
         <v>113</v>
       </c>
       <c r="F22" s="14"/>
-      <c r="G22" s="21"/>
+      <c r="G22" s="22"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
@@ -2053,7 +2065,7 @@
         <v>113</v>
       </c>
       <c r="F23" s="16"/>
-      <c r="G23" s="22"/>
+      <c r="G23" s="23"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">

</xml_diff>